<commit_message>
Tested User Add Stock!
</commit_message>
<xml_diff>
--- a/Users/Testing.xlsx
+++ b/Users/Testing.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,21 +472,46 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>200</v>
+        <v>600</v>
       </c>
       <c r="C2" t="n">
-        <v>123.81</v>
+        <v>118.4</v>
       </c>
       <c r="D2" t="n">
-        <v>123.81</v>
+        <v>118.4</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.43</v>
+        <v>-4.78</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.54</v>
+        <v>-5.95</v>
       </c>
       <c r="G2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>UNITYR3</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>7500</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="E3" t="n">
+        <v>55.65</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="G3" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>